<commit_message>
css page confirmation + fin du plan test
</commit_message>
<xml_diff>
--- a/plan test.xlsx
+++ b/plan test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mouatakide1\Desktop\Projet 5\souadmouatakide_5_09032021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6992C1-FF74-430A-AD52-CC0663A8C3DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E1B232-9A89-4777-9373-5ACD4EB88C93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="150" yWindow="0" windowWidth="19050" windowHeight="14760" xr2:uid="{2878A0D4-6779-429E-8553-B62F99789558}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="113">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -314,6 +314,57 @@
   </si>
   <si>
     <t>Plan de test "Orinoco"</t>
+  </si>
+  <si>
+    <t>confirmation.js</t>
+  </si>
+  <si>
+    <t>orderId</t>
+  </si>
+  <si>
+    <t>Affiche le numéro de commande dans la console</t>
+  </si>
+  <si>
+    <t>console.log(orderId);</t>
+  </si>
+  <si>
+    <t>N'affiche pas le numéro de commande</t>
+  </si>
+  <si>
+    <t>messageDeConfirmation</t>
+  </si>
+  <si>
+    <t>Affiche un message de confirmation avec le numéro de commande</t>
+  </si>
+  <si>
+    <t>n'affiche pas de message</t>
+  </si>
+  <si>
+    <t>Si le message apparait sur le site, la commande est confirmée</t>
+  </si>
+  <si>
+    <t>PrixConfirm</t>
+  </si>
+  <si>
+    <t>9-10</t>
+  </si>
+  <si>
+    <t>Affiche un message avec le prix total de la commande</t>
+  </si>
+  <si>
+    <t>Si le message apparait sur le site, le prix est confirmée</t>
+  </si>
+  <si>
+    <t>ordreDeConfirmation()</t>
+  </si>
+  <si>
+    <t>2-13</t>
+  </si>
+  <si>
+    <t>Affichage d'un message de confirmation avec prix total de la commande</t>
+  </si>
+  <si>
+    <t>si un message de confirmation avec le prix de la commande s'affiche sur le site, la commande est confirmée, sinon n'affiche rien</t>
   </si>
 </sst>
 </file>
@@ -359,7 +410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -428,20 +479,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -473,24 +515,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -506,10 +530,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -517,6 +544,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -845,13 +881,13 @@
   </sheetPr>
   <dimension ref="A1:F419"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.140625" customWidth="1"/>
@@ -860,22 +896,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -978,64 +1014,64 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="16" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="12"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="12"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="13"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1147,13 +1183,13 @@
       <c r="C18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="16" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1167,23 +1203,23 @@
       <c r="C19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="11" t="s">
         <v>72</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -1195,9 +1231,9 @@
       <c r="C21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -1209,9 +1245,9 @@
       <c r="C22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -1293,165 +1329,213 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
+      <c r="A45" s="14"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
+      <c r="A46" s="14"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>

</xml_diff>

<commit_message>
plan test a refaire
</commit_message>
<xml_diff>
--- a/plan test.xlsx
+++ b/plan test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mouatakide1\Desktop\Projet 5\souadmouatakide_5_09032021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smoua\Dropbox\Mon PC (LAPTOP-CEI78QN6)\Desktop\projet5\souadmouatakide_5_09032021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E1B232-9A89-4777-9373-5ACD4EB88C93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE81556-C1A3-483A-9EA2-95D31932A59F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="150" yWindow="0" windowWidth="19050" windowHeight="14760" xr2:uid="{2878A0D4-6779-429E-8553-B62F99789558}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="103">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -54,24 +54,9 @@
     <t>3</t>
   </si>
   <si>
-    <t>URL API</t>
-  </si>
-  <si>
-    <t>vérification de la visibilité de l'url api</t>
-  </si>
-  <si>
-    <t>console.log(URLAPI);</t>
-  </si>
-  <si>
-    <t>url api mal orthopraphiée</t>
-  </si>
-  <si>
     <t>15-41</t>
   </si>
   <si>
-    <t>insertProduit(data)</t>
-  </si>
-  <si>
     <t>console.log(data);</t>
   </si>
   <si>
@@ -82,63 +67,6 @@
   </si>
   <si>
     <t>3-9</t>
-  </si>
-  <si>
-    <t>Retourne un tableau de tous les éléments</t>
-  </si>
-  <si>
-    <t>Renvoie l'élément correspondant à identifiant given_id</t>
-  </si>
-  <si>
-    <t>console.log(iD);</t>
-  </si>
-  <si>
-    <t>Ne retourne pas de tableau</t>
-  </si>
-  <si>
-    <t>l'identifiant du produit ne s'affiche pas</t>
-  </si>
-  <si>
-    <t>listeColor</t>
-  </si>
-  <si>
-    <t>52-57</t>
-  </si>
-  <si>
-    <t>retourne une liste d'option de couleur</t>
-  </si>
-  <si>
-    <t>console.log(listeColor);</t>
-  </si>
-  <si>
-    <t>la liste d'option ne s'affiche pas</t>
-  </si>
-  <si>
-    <t>panier</t>
-  </si>
-  <si>
-    <t>59-72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transmission de l'article dans le localstorage </t>
-  </si>
-  <si>
-    <t>                    window.location.href = "Panier.html";</t>
-  </si>
-  <si>
-    <t>                } else {</t>
-  </si>
-  <si>
-    <t>                    window.location.href = "../index.html";</t>
-  </si>
-  <si>
-    <t>                }</t>
-  </si>
-  <si>
-    <t>if(window.confirm("Article bien ajouté au panier.                           Souhaitez vous consulter votre panier ?")){</t>
-  </si>
-  <si>
-    <t>l'article n'est pas stocké dans le localstorage</t>
   </si>
   <si>
     <t>affichageLocalStoragePanier</t>
@@ -365,6 +293,48 @@
   </si>
   <si>
     <t>si un message de confirmation avec le prix de la commande s'affiche sur le site, la commande est confirmée, sinon n'affiche rien</t>
+  </si>
+  <si>
+    <t>récupération de la liste de produit à la vente</t>
+  </si>
+  <si>
+    <t>console.log(Produit());</t>
+  </si>
+  <si>
+    <t>Produit()</t>
+  </si>
+  <si>
+    <t>data incorrect</t>
+  </si>
+  <si>
+    <t>insert les produit fourni dans le data dans l'HTML</t>
+  </si>
+  <si>
+    <t>Appeler la fonction insert produit avec différente valeur du data</t>
+  </si>
+  <si>
+    <t>insertProduit(data) data est untableau de produit disponible</t>
+  </si>
+  <si>
+    <t>récupére le parametre d'url Id, ajoute le valeur à la variable Idproduct et appel la fonction produit en lui transmettant au paramètre Id</t>
+  </si>
+  <si>
+    <t>en transmttant des paramètre url et console.log(iD)</t>
+  </si>
+  <si>
+    <t>pas de parmetre id transmit dans url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produit(iD) </t>
+  </si>
+  <si>
+    <t>récupération des info id d'un produit et appel de la fonction insert product et en lui transmettant en paramètre le tableau des donner</t>
+  </si>
+  <si>
+    <t>appeler la fonction produit() en lui transmettant les id</t>
+  </si>
+  <si>
+    <t>id invalide</t>
   </si>
 </sst>
 </file>
@@ -483,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -554,6 +524,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,7 +553,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -881,11 +854,11 @@
   </sheetPr>
   <dimension ref="A1:F419"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:F30"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
@@ -897,7 +870,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -941,106 +914,86 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="A8" s="16"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="22"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="E9" s="8"/>
       <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1048,9 +1001,7 @@
       <c r="B10" s="22"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="E10" s="8"/>
       <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1058,9 +1009,7 @@
       <c r="B11" s="22"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="E11" s="8"/>
       <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1068,9 +1017,7 @@
       <c r="B12" s="23"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
-      <c r="E12" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="E12" s="7"/>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1078,19 +1025,19 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1098,19 +1045,19 @@
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1118,19 +1065,19 @@
         <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1138,19 +1085,19 @@
         <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1158,19 +1105,19 @@
         <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1178,19 +1125,19 @@
         <v>7</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1198,10 +1145,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -1212,10 +1159,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -1226,10 +1173,10 @@
         <v>7</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -1240,10 +1187,10 @@
         <v>7</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
@@ -1254,19 +1201,19 @@
         <v>7</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1274,19 +1221,19 @@
         <v>7</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1294,19 +1241,19 @@
         <v>7</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1314,99 +1261,99 @@
         <v>7</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
modification du plan test
</commit_message>
<xml_diff>
--- a/plan test.xlsx
+++ b/plan test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smoua\Dropbox\Mon PC (LAPTOP-CEI78QN6)\Desktop\projet5\souadmouatakide_5_09032021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mouatakide1\Desktop\Projet 5\souadmouatakide_5_09032021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE81556-C1A3-483A-9EA2-95D31932A59F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652E1BAE-029D-4086-A4E3-B16B9B9289C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="150" yWindow="0" windowWidth="19050" windowHeight="14760" xr2:uid="{2878A0D4-6779-429E-8553-B62F99789558}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -51,290 +51,151 @@
     <t>panier.js</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>15-41</t>
   </si>
   <si>
-    <t>console.log(data);</t>
-  </si>
-  <si>
-    <t>getId</t>
-  </si>
-  <si>
     <t>article.js</t>
   </si>
   <si>
     <t>3-9</t>
   </si>
   <si>
-    <t>affichageLocalStoragePanier</t>
-  </si>
-  <si>
-    <t>5-6</t>
-  </si>
-  <si>
-    <t>getProduitsPaniers</t>
-  </si>
-  <si>
-    <t>console.log('articles mis au panier');</t>
-  </si>
-  <si>
     <t>9-19</t>
   </si>
   <si>
-    <t>retourne un nombre d'article stocké dans le localstorage</t>
-  </si>
-  <si>
-    <t>Ne retourne pas d'article dansle localstorage</t>
-  </si>
-  <si>
-    <t>retourne un tableau d'id stocké dans le localstorage</t>
-  </si>
-  <si>
-    <t>console.log(affichageLocalStoragePanier);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ne retoune pas de tableau </t>
-  </si>
-  <si>
     <t>insertPanier(data, i)</t>
   </si>
   <si>
-    <t>Retroune un objet contenant toute les informations de l'article</t>
-  </si>
-  <si>
-    <t>Ne retourne pas d'article</t>
-  </si>
-  <si>
-    <t>35-72</t>
-  </si>
-  <si>
     <t>supprimerProduit(j)</t>
   </si>
   <si>
-    <t>Suppression d'un article</t>
-  </si>
-  <si>
-    <t>alert("cet article va etre suprimé!");</t>
-  </si>
-  <si>
-    <t>L'article n'est pas supprimé</t>
-  </si>
-  <si>
     <t>59-65</t>
   </si>
   <si>
-    <t>Affichage du prix total dans la page du site</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t> console.log(total);</t>
-  </si>
-  <si>
-    <t>le total ne s'affiche pas</t>
-  </si>
-  <si>
-    <t>68-71</t>
-  </si>
-  <si>
-    <t>184-195</t>
-  </si>
-  <si>
-    <t>validName</t>
-  </si>
-  <si>
-    <t>return true lorsque c'est bon et return false lorsque c'est faux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">le texte avec les couleurs ne s'affiche pas </t>
-  </si>
-  <si>
-    <t>validFirstName</t>
-  </si>
-  <si>
-    <t>validAdresse</t>
-  </si>
-  <si>
-    <t>validCity</t>
-  </si>
-  <si>
-    <t>validEmail</t>
-  </si>
-  <si>
-    <t>221-232</t>
-  </si>
-  <si>
-    <t>296-307</t>
-  </si>
-  <si>
-    <t>259-270</t>
-  </si>
-  <si>
-    <t>319-330</t>
-  </si>
-  <si>
-    <t>Affichage d'un texte en rouge si l'expression régulière n'est pas respecté et le texte s'affiche en vert lorsque la zone est bien rempli</t>
-  </si>
-  <si>
     <t>formulaire.addEventListener</t>
   </si>
   <si>
     <t>97-137</t>
   </si>
   <si>
-    <t>Redirection vers la page de confirmation</t>
-  </si>
-  <si>
-    <t>si le formulaire est bien rempli: window.location.href = "confirmation.html"; console.log('le formulaire est valide'); et si le formulaire est mal rempli: console.log("le formulaire est incorrect");
-        alert("veuillez remplir le formulaire pour valider la commande...");</t>
-  </si>
-  <si>
-    <t>la page panier reste, la redirection ne se fait pas</t>
-  </si>
-  <si>
-    <t>object</t>
-  </si>
-  <si>
-    <t>option</t>
-  </si>
-  <si>
-    <t>response.orderId</t>
-  </si>
-  <si>
-    <t>console.log(response.orderId);</t>
-  </si>
-  <si>
-    <t>Renvoie le numéro de commande</t>
-  </si>
-  <si>
-    <t>ne renvoie pas de numéro de commande</t>
-  </si>
-  <si>
-    <t>123-129</t>
-  </si>
-  <si>
-    <t>console.log(object);</t>
-  </si>
-  <si>
-    <t>console.log(option);</t>
-  </si>
-  <si>
-    <t>109-111</t>
-  </si>
-  <si>
-    <t>113-119</t>
-  </si>
-  <si>
-    <t>Affiche dans la console un objet avec un tableau de produit qui se trouve dans le localstorage</t>
-  </si>
-  <si>
-    <t>N'affiche pas d'objet ni de produit</t>
-  </si>
-  <si>
-    <t>Affiche dans la console un objet avec un nouveau constructor d'objet pour avoir un numéro de commande unique</t>
-  </si>
-  <si>
-    <t>N'affiche pas le nouveau objet constructor et ne génére pas de numéro de commande</t>
-  </si>
-  <si>
     <t>Plan de test "Orinoco"</t>
   </si>
   <si>
     <t>confirmation.js</t>
   </si>
   <si>
-    <t>orderId</t>
-  </si>
-  <si>
-    <t>Affiche le numéro de commande dans la console</t>
-  </si>
-  <si>
-    <t>console.log(orderId);</t>
-  </si>
-  <si>
-    <t>N'affiche pas le numéro de commande</t>
-  </si>
-  <si>
-    <t>messageDeConfirmation</t>
-  </si>
-  <si>
-    <t>Affiche un message de confirmation avec le numéro de commande</t>
-  </si>
-  <si>
-    <t>n'affiche pas de message</t>
-  </si>
-  <si>
-    <t>Si le message apparait sur le site, la commande est confirmée</t>
-  </si>
-  <si>
-    <t>PrixConfirm</t>
-  </si>
-  <si>
-    <t>9-10</t>
-  </si>
-  <si>
-    <t>Affiche un message avec le prix total de la commande</t>
-  </si>
-  <si>
-    <t>Si le message apparait sur le site, le prix est confirmée</t>
-  </si>
-  <si>
     <t>ordreDeConfirmation()</t>
   </si>
   <si>
     <t>2-13</t>
   </si>
   <si>
-    <t>Affichage d'un message de confirmation avec prix total de la commande</t>
-  </si>
-  <si>
-    <t>si un message de confirmation avec le prix de la commande s'affiche sur le site, la commande est confirmée, sinon n'affiche rien</t>
-  </si>
-  <si>
-    <t>récupération de la liste de produit à la vente</t>
-  </si>
-  <si>
     <t>console.log(Produit());</t>
   </si>
   <si>
     <t>Produit()</t>
   </si>
   <si>
-    <t>data incorrect</t>
-  </si>
-  <si>
-    <t>insert les produit fourni dans le data dans l'HTML</t>
-  </si>
-  <si>
-    <t>Appeler la fonction insert produit avec différente valeur du data</t>
-  </si>
-  <si>
-    <t>insertProduit(data) data est untableau de produit disponible</t>
-  </si>
-  <si>
-    <t>récupére le parametre d'url Id, ajoute le valeur à la variable Idproduct et appel la fonction produit en lui transmettant au paramètre Id</t>
-  </si>
-  <si>
-    <t>en transmttant des paramètre url et console.log(iD)</t>
-  </si>
-  <si>
-    <t>pas de parmetre id transmit dans url</t>
-  </si>
-  <si>
     <t xml:space="preserve">Produit(iD) </t>
   </si>
   <si>
-    <t>récupération des info id d'un produit et appel de la fonction insert product et en lui transmettant en paramètre le tableau des donner</t>
-  </si>
-  <si>
-    <t>appeler la fonction produit() en lui transmettant les id</t>
-  </si>
-  <si>
-    <t>id invalide</t>
+    <t>5-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La fonction n'admet aucun paramètre mais va utiliser dans un fetch ma variable "let URLAPI"  afin de récupérer une liste de produit disponible à la vente </t>
+  </si>
+  <si>
+    <t>L'API ne répond ou l'URL d'API est incorrect ou bien il n'y a pas de produit disponible à la vente</t>
+  </si>
+  <si>
+    <t>La fonction doit pouvoir injecter les produits fournis dans data dans l'HTML</t>
+  </si>
+  <si>
+    <t>Créer une fonction qui appel la fonction insertproduit() en transmettant différente valeur du data</t>
+  </si>
+  <si>
+    <t>le tableau data est incorrect donc aucun affichage HTML</t>
+  </si>
+  <si>
+    <t>insertProduit(data) data est un tableau d'objet de produit disponible à la vente.Pour le faire fonctionner on à besoin des champs: data.imageURL,data.name et data.price</t>
+  </si>
+  <si>
+    <t>La fonction récupère le pramètre d'URL "iD" transmis dans l'URL. Elle ajoute la valeur à ma variable idProduct et elle appelle ma fonction Produit()en transmettant en paramètre Id</t>
+  </si>
+  <si>
+    <t>getId()</t>
+  </si>
+  <si>
+    <t>En transmettant diffèrents paramètres d'URL et appeler getId en faisant un console.log(iD)</t>
+  </si>
+  <si>
+    <t>Il n'y a pas de paramètre iD qui est transmis dans l'URL</t>
+  </si>
+  <si>
+    <t>13-20</t>
+  </si>
+  <si>
+    <t>Elle récupère les informations iD d'un produit pour l'iD donné, elle appelle la fonction insertProduct() et en lui transmettant en paramètre le tableau des données récupérées</t>
+  </si>
+  <si>
+    <t>Appeler la fonction Produit() en lui transmettant différents iD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'iD de produit n'existe pas </t>
+  </si>
+  <si>
+    <t>22-71</t>
+  </si>
+  <si>
+    <t>Elle affiche ou non le formulaire. En vérifiant si des produits sont stockés dans le localstorage, si le localstorage est vide elle cahe le formulaire et affiche un message dans l'HTML et s'il y a des produits, elle va faire une boucle pour parcourir l'ensemble des élèments stockés dans le localstorage puis elle appelle la fonction Produit(iD)</t>
+  </si>
+  <si>
+    <t>getProduitsPanier()</t>
+  </si>
+  <si>
+    <t>21-31</t>
+  </si>
+  <si>
+    <t>Produit(iD, i)</t>
+  </si>
+  <si>
+    <t>34-71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La fonction doit pouvoir injecter les produits fournis dans data dans l'HTML </t>
+  </si>
+  <si>
+    <t xml:space="preserve">insertProduit(data) </t>
+  </si>
+  <si>
+    <t>Si le formulaire est valide il y aura une redirection vers la page commande sinon une alerte va s'afficher sur la page panier. On peut faire un console.log(response.orderId); pour obtenir le numéro de commande.</t>
+  </si>
+  <si>
+    <t>Il n'y aura pas de numéro de commande et la page restera bloquée sur la page panier</t>
+  </si>
+  <si>
+    <t>nom.addEventListener</t>
+  </si>
+  <si>
+    <t>prenom.addEventListener</t>
+  </si>
+  <si>
+    <t>email.addEventListener</t>
+  </si>
+  <si>
+    <t>adresse.addEventListener</t>
+  </si>
+  <si>
+    <t>ville.addEventListener</t>
+  </si>
+  <si>
+    <t>Il y a un écouteur d'évenement pour chaque fonction qui va observer le changement pour chaque étape du formulaire et chaque input est associé à une variable de validation qui va être testé dans la fonction du formulaire.addEventListener</t>
+  </si>
+  <si>
+    <t>le formulaire ne sera pas testé car l'écouteur d'évenement n'aura pas fonctionné</t>
+  </si>
+  <si>
+    <t>Va traiter le formulaire, il y a un écouteur d'évenement sur le formulaire à chaque click. Elle va tester chacun de mes champs input , va construire l'objet qui va être envoyé, et va faire une requette auprès de l'API pour obtenir un numéro de commande afin de pouvoir envoyer les informations de la commande vers la page commande, elle va attendre la réponse. si elle est valide  il y aura une redirection et une suppression du panier sinon il y aura un message d'alerte</t>
   </si>
 </sst>
 </file>
@@ -453,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -476,18 +337,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -499,6 +348,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -522,9 +377,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -553,7 +405,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -852,39 +704,39 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F419"/>
+  <dimension ref="A1:F418"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" customWidth="1"/>
     <col min="5" max="5" width="61.140625" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="A1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -906,583 +758,472 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>99</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>100</v>
+        <v>36</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="16"/>
+      <c r="A8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="17"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="17"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="17"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="18"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:6" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" ht="170.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>41</v>
+      <c r="C18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+        <v>50</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>48</v>
-      </c>
+      <c r="B20" s="4"/>
       <c r="C20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+        <v>51</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="B21" s="4"/>
       <c r="C21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>49</v>
-      </c>
+      <c r="B22" s="4"/>
       <c r="C22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>79</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
+      <c r="A46" s="1"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
@@ -1742,7 +1483,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
-      <c r="B79" s="5"/>
+      <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -4460,25 +4201,18 @@
       <c r="E418" s="1"/>
       <c r="F418" s="1"/>
     </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A419" s="1"/>
-      <c r="B419" s="1"/>
-      <c r="C419" s="1"/>
-      <c r="D419" s="1"/>
-      <c r="E419" s="1"/>
-      <c r="F419" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="E18:E22"/>
-    <mergeCell ref="F18:F22"/>
+  <mergeCells count="10">
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="D8:D12"/>
     <mergeCell ref="C8:C12"/>
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="F8:F12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="E18:E22"/>
+    <mergeCell ref="F18:F22"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
minimisation de la page panier
</commit_message>
<xml_diff>
--- a/plan test.xlsx
+++ b/plan test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mouatakide1\Desktop\Projet 5\souadmouatakide_5_09032021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F095F22-34BB-44A9-9E27-1C2037C67E06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F40374-12E7-46D5-8DF5-F53D050C7367}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="0" windowWidth="19050" windowHeight="14760" xr2:uid="{2878A0D4-6779-429E-8553-B62F99789558}"/>
+    <workbookView xWindow="150" yWindow="600" windowWidth="19050" windowHeight="14760" xr2:uid="{2878A0D4-6779-429E-8553-B62F99789558}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -51,69 +51,21 @@
     <t>panier.js</t>
   </si>
   <si>
-    <t>15-41</t>
-  </si>
-  <si>
     <t>article.js</t>
   </si>
   <si>
-    <t>3-9</t>
-  </si>
-  <si>
-    <t>9-19</t>
-  </si>
-  <si>
-    <t>insertPanier(data, i)</t>
-  </si>
-  <si>
-    <t>supprimerProduit(j)</t>
-  </si>
-  <si>
-    <t>59-65</t>
-  </si>
-  <si>
-    <t>formulaire.addEventListener</t>
-  </si>
-  <si>
-    <t>97-137</t>
-  </si>
-  <si>
     <t>Plan de test "Orinoco"</t>
   </si>
   <si>
     <t>confirmation.js</t>
   </si>
   <si>
-    <t>ordreDeConfirmation()</t>
-  </si>
-  <si>
-    <t>2-13</t>
-  </si>
-  <si>
-    <t>console.log(Produit());</t>
-  </si>
-  <si>
-    <t>Produit()</t>
-  </si>
-  <si>
     <t xml:space="preserve">Produit(iD) </t>
   </si>
   <si>
-    <t>5-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La fonction n'admet aucun paramètre mais va utiliser dans un fetch ma variable "let URLAPI"  afin de récupérer une liste de produit disponible à la vente </t>
-  </si>
-  <si>
-    <t>L'API ne répond ou l'URL d'API est incorrect ou bien il n'y a pas de produit disponible à la vente</t>
-  </si>
-  <si>
     <t>le tableau data est incorrect donc aucun affichage HTML</t>
   </si>
   <si>
-    <t>insertProduit(data) data est un tableau d'objet de produit disponible à la vente.Pour le faire fonctionner on à besoin des champs: data.imageURL,data.name et data.price</t>
-  </si>
-  <si>
     <t>La fonction récupère le pramètre d'URL "iD" transmis dans l'URL. Elle ajoute la valeur à ma variable idProduct et elle appelle ma fonction Produit()en transmettant en paramètre Id</t>
   </si>
   <si>
@@ -126,12 +78,6 @@
     <t>Il n'y a pas de paramètre iD qui est transmis dans l'URL</t>
   </si>
   <si>
-    <t>13-20</t>
-  </si>
-  <si>
-    <t>Elle récupère les informations iD d'un produit pour l'iD donné, elle appelle la fonction insertProduct() et en lui transmettant en paramètre le tableau des données récupérées</t>
-  </si>
-  <si>
     <t>Appeler la fonction Produit() en lui transmettant différents iD</t>
   </si>
   <si>
@@ -141,70 +87,10 @@
     <t>22-71</t>
   </si>
   <si>
-    <t>Elle affiche ou non le formulaire. En vérifiant si des produits sont stockés dans le localstorage, si le localstorage est vide elle cahe le formulaire et affiche un message dans l'HTML et s'il y a des produits, elle va faire une boucle pour parcourir l'ensemble des élèments stockés dans le localstorage puis elle appelle la fonction Produit(iD)</t>
-  </si>
-  <si>
-    <t>getProduitsPanier()</t>
-  </si>
-  <si>
-    <t>21-31</t>
-  </si>
-  <si>
-    <t>Produit(iD, i)</t>
-  </si>
-  <si>
-    <t>34-71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La fonction doit pouvoir injecter les produits fournis dans data dans l'HTML </t>
-  </si>
-  <si>
     <t>Si le formulaire est valide il y aura une redirection vers la page commande sinon une alerte va s'afficher sur la page panier. On peut faire un console.log(response.orderId); pour obtenir le numéro de commande.</t>
   </si>
   <si>
     <t>Il n'y aura pas de numéro de commande et la page restera bloquée sur la page panier</t>
-  </si>
-  <si>
-    <t>nom.addEventListener</t>
-  </si>
-  <si>
-    <t>prenom.addEventListener</t>
-  </si>
-  <si>
-    <t>email.addEventListener</t>
-  </si>
-  <si>
-    <t>adresse.addEventListener</t>
-  </si>
-  <si>
-    <t>ville.addEventListener</t>
-  </si>
-  <si>
-    <t>Il y a un écouteur d'évenement pour chaque fonction qui va observer le changement pour chaque étape du formulaire et chaque input est associé à une variable de validation qui va être testé dans la fonction du formulaire.addEventListener</t>
-  </si>
-  <si>
-    <t>le formulaire ne sera pas testé car l'écouteur d'évenement n'aura pas fonctionné</t>
-  </si>
-  <si>
-    <t>Va traiter le formulaire, il y a un écouteur d'évenement sur le formulaire à chaque click. Elle va tester chacun de mes champs input , va construire l'objet qui va être envoyé, et va faire une requette auprès de l'API pour obtenir un numéro de commande afin de pouvoir envoyer les informations de la commande vers la page commande, elle va attendre la réponse. si elle est valide  il y aura une redirection et une suppression du panier sinon il y aura un message d'alerte</t>
-  </si>
-  <si>
-    <t>validName</t>
-  </si>
-  <si>
-    <t>validFirstName</t>
-  </si>
-  <si>
-    <t>validAdresse</t>
-  </si>
-  <si>
-    <t>validCity </t>
-  </si>
-  <si>
-    <t>validEmail</t>
-  </si>
-  <si>
-    <t>Une condition avec un regex est appliquée pour chaque fonction afin de contrôler le déroulement du formulaire, puis une autre condition va tester l'expression régulière</t>
   </si>
   <si>
     <t>Appeler la fonction avec différentes
@@ -212,52 +98,128 @@
 minuscules...)</t>
   </si>
   <si>
-    <t>La valeur retournée pourrait être érronée</t>
-  </si>
-  <si>
-    <t>insertProduit(data) data est un tableau d'objet de produit disponible à la vente.Pour le faire fonctionner on a besoin des champs: data.imageUrl, data.name, data.price, data.description et data.colors[i]</t>
-  </si>
-  <si>
-    <t>Créer une fonction qui appel la fonction insertProduit() en transmettant différente valeur du data</t>
-  </si>
-  <si>
-    <t>La fonction doit pouvoir injecter les produits fournis dans data , dans l'HTML. Elle doit nous permettre de séléctionner une couleur dans les options et ajouter au click le produit dans le localstorage</t>
-  </si>
-  <si>
     <t>Créer une fonction qui appel la fonction insertProduit() en transmettant différente valeur du data. Et lors du click sur le bouton ajouter un message de confirmation apparaitra avec une redirection dans la page index si on veut continuer les achats ou dans la page panier</t>
   </si>
   <si>
-    <t>on aura les produit afficher dans l'HTML si on a séléctionné des produit , sinon il y aura un message sur l'HTML si le panier est vide</t>
-  </si>
-  <si>
-    <t>il n'y aura pas d'affichage sur l'HTML</t>
-  </si>
-  <si>
-    <t>Créer une fonction qui appel la fonction insertProduit() en transmettant différente valeur du data, on peut ajouter des produits pour montrer que le prix total fait bien le calcule des prix.</t>
-  </si>
-  <si>
-    <t>le tableau data est incorrect donc aucun affichage HTML, le total ne calcule pas bien les prix des produits</t>
-  </si>
-  <si>
-    <t>supprimer un produit affiché</t>
-  </si>
-  <si>
-    <t>Elle récupère l'écouteur d'évenement qui est dans la fonction insertPanier ( ) , elle permet de retirer un produit dans le localstorage, de faire la mise à jour du localostorage, et regarge la page de l'application</t>
-  </si>
-  <si>
-    <t>La fonction doit pouvoir injecter les produits fournis dans data , dans l'HTML, Il y a une variable qui calcule de prix total des produits contenus dans le localstorage et il y a une boucle for avec un écouteur d'évenement qui va etre utilisé pour la fonction  supprimerProduit(j) avec un message d'alerte lorsque le produit est supprimé.</t>
-  </si>
-  <si>
     <t>Le produit ne se supprime pas</t>
   </si>
   <si>
-    <t>elle permet de récupérer le numéro de commande et le prix total stocké dans le localstorage, elle inject dans l'HTML un message de confirmation avec le total.</t>
-  </si>
-  <si>
     <t>La valeur retournée pourrait ne pas correspondre au résultat attendu</t>
   </si>
   <si>
-    <t xml:space="preserve">Modifier la commande </t>
+    <t>5-41</t>
+  </si>
+  <si>
+    <t>function() fonction anonyme qui comprend un fetch, et un tableau d'objet de produit disponible à la vente.Pour le faire fonctionner on à besoin des champs: response[i]._id, response[i].imageUrl, response[i].name, response[i].price</t>
+  </si>
+  <si>
+    <t>La fonction n'admet aucun paramètre mais va utiliser dans un premier temps, un fetch ma variable "let URLAPI" . La requête doit retourner une promesse (response) contenant tous les produits et leurs spécifications sous forme de tableau d'objets. Puis doit pouvoir injecter les produits fournis dans l'HTML .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le résultat de la requête doit afficher la liste des produits sous forme de liste. Je peux vérifier avec un console.log(response).  Les 5 objets contenant les informations sur chacun des produits doivent apparaitre dans la console; La page d'accueil doit afficher la liste de tous les éléments du tableau, leurs spécifications ainsi qu'un lien permettant d'accéder à la page produit de l'ours sélectionné. </t>
+  </si>
+  <si>
+    <t>L'API ne répond ou l'URL d'API est incorrect ou bien il n'y a pas de produit disponible à la vente; le tableau response est incorrect donc aucun affichage HTML</t>
+  </si>
+  <si>
+    <t>5-11</t>
+  </si>
+  <si>
+    <t>13-23</t>
+  </si>
+  <si>
+    <t>Cette fonction doit retourner une promesse (response) qui contient chaque élément de l'API. Cette réponse est retournée sous forme d'objets (id) qui contient les spécifications et un tableau des différentes couleurs pour chacun des produits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insertProduit(data) data est un tableau d'objet de produit disponible à la vente.Pour le faire fonctionner on a besoin des champs: response.imageUrl, response.name, response.price / 100, response.description, response.colors[i] </t>
+  </si>
+  <si>
+    <t>La fonction doit pouvoir injecter les produits fournis dans response , dans l'HTML. Elle doit nous permettre de séléctionner une couleur dans les options et ajouter au click le produit dans le localstorage</t>
+  </si>
+  <si>
+    <t>generateCart(cart)</t>
+  </si>
+  <si>
+    <t>Elle affiche ou non le formulaire. En vérifiant si des produits sont stockés dans le localstorage, si le localstorage est vide elle cahe le formulaire et affiche un message dans l'HTML et s'il y a des produits, elle va faire une boucle pour parcourir l'ensemble des élèments stockés dans le localstorage,La fonction doit pouvoir injecter les produits fournis dans response , dans l'HTML, Il y a une variable qui calcule le prix total des produits contenus dans le localstorage. la fonction va appeler la fonction generateForm() pour transmettre les informations.</t>
+  </si>
+  <si>
+    <t>on aura les produit afficher dans l'HTML si on a séléctionné des produits , sinon il y aura un message sur l'HTML si le panier est vide.On peut ajouter des produits pour montrer que le prix total fait bien le calcule des prix.</t>
+  </si>
+  <si>
+    <t>il n'y aura pas d'affichage sur l'HTML; le tableau response est incorrect donc aucun affichage HTML, le total ne calcule pas bien les prix des produits</t>
+  </si>
+  <si>
+    <t>6-38</t>
+  </si>
+  <si>
+    <t>clickOnDelete(i)</t>
+  </si>
+  <si>
+    <t>42-46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette fonction permet de supprimer un des produits affichés dans le panier </t>
+  </si>
+  <si>
+    <t>function()</t>
+  </si>
+  <si>
+    <t>48-52</t>
+  </si>
+  <si>
+    <t>cette fonction anonyme permet de parcourir le tableau des produits présents dans le localstorage et de créer un écouteur d'évenement qui appel la fonction clikOnDelete(i)</t>
+  </si>
+  <si>
+    <t>supprimer un produit affiché, une alerte va s'afficher pour prévenir de la suppression du produit</t>
+  </si>
+  <si>
+    <t>checktext(text,email)</t>
+  </si>
+  <si>
+    <t>59-70</t>
+  </si>
+  <si>
+    <t>Des conditions avec une regex est testés afin de contrôler le déroulement du formulaire au niveau de l'email.</t>
+  </si>
+  <si>
+    <t>Appeler la fonction avec différentes
+valeurs de tests (des chiffres, des lettres, des lettres majuscules, des caractères spéciaux)si l'email entré ne correspond pas à la regex il y aura une alerte et return false, sinon elle return true</t>
+  </si>
+  <si>
+    <t>La regex ne fonctionne pas</t>
+  </si>
+  <si>
+    <t>73-116</t>
+  </si>
+  <si>
+    <t>generateForm()</t>
+  </si>
+  <si>
+    <t>Cette fonction permet la création du formulaire de contact, elle va vérifier les champs input du nom, prenom, email, ville et adresse avec un écouteur d'événement.  Elle va bloquer l'execution du formulaire si les vérifications ne donnent pas de résultats conformes. Et elle va envoyer l'object contact si les vérifications donnent des résultats conformes à la fonction sendOrder(contact).</t>
+  </si>
+  <si>
+    <t>Le formulaire ne réagit pas</t>
+  </si>
+  <si>
+    <t>sendOrder(contact)</t>
+  </si>
+  <si>
+    <t>142-166</t>
+  </si>
+  <si>
+    <t>Cette fonction doit envoyer au serveur l'élément passé en paramètre (ici la commande contenant le panier et les données du formulaire) et recevoir la réponse du serveur (le numéro de confirmation de la commande). Elle va retourner un numéro de commande, puis envoyer la réponse(numéro de commande) vers la page commande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function () </t>
+  </si>
+  <si>
+    <t>3-18</t>
+  </si>
+  <si>
+    <t>Modifier la commande pour voir un nouveau numéro de commande et un nouveau prix</t>
+  </si>
+  <si>
+    <t>Cette fonction doit afficher le numéro de la confirmation de la commande sur la page commande ainsi que le total des achats, pui elle va supprimer les produits stockés dans le localStorage</t>
   </si>
 </sst>
 </file>
@@ -376,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -396,9 +358,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -411,19 +370,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -432,13 +394,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -766,10 +722,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F417"/>
+  <dimension ref="A1:F408"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +740,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -820,514 +776,461 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="B6" s="4" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="19" t="s">
+      <c r="D12" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="1:6" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="E12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>69</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="170.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="C19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+        <v>60</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-    </row>
-    <row r="22" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>61</v>
-      </c>
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
+      <c r="A40" s="1"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
+      <c r="A41" s="1"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
+      <c r="A43" s="1"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
+      <c r="A44" s="1"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
@@ -1523,7 +1426,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-      <c r="B69" s="5"/>
+      <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -1531,7 +1434,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="B70" s="5"/>
+      <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -1539,7 +1442,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
-      <c r="B71" s="5"/>
+      <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -1547,7 +1450,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
-      <c r="B72" s="5"/>
+      <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -1555,7 +1458,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="B73" s="5"/>
+      <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -1563,7 +1466,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
-      <c r="B74" s="5"/>
+      <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -1571,7 +1474,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="B75" s="5"/>
+      <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -1579,7 +1482,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
-      <c r="B76" s="5"/>
+      <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -1587,7 +1490,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
-      <c r="B77" s="5"/>
+      <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -4241,93 +4144,23 @@
       <c r="E408" s="1"/>
       <c r="F408" s="1"/>
     </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A409" s="1"/>
-      <c r="B409" s="1"/>
-      <c r="C409" s="1"/>
-      <c r="D409" s="1"/>
-      <c r="E409" s="1"/>
-      <c r="F409" s="1"/>
-    </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A410" s="1"/>
-      <c r="B410" s="1"/>
-      <c r="C410" s="1"/>
-      <c r="D410" s="1"/>
-      <c r="E410" s="1"/>
-      <c r="F410" s="1"/>
-    </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A411" s="1"/>
-      <c r="B411" s="1"/>
-      <c r="C411" s="1"/>
-      <c r="D411" s="1"/>
-      <c r="E411" s="1"/>
-      <c r="F411" s="1"/>
-    </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A412" s="1"/>
-      <c r="B412" s="1"/>
-      <c r="C412" s="1"/>
-      <c r="D412" s="1"/>
-      <c r="E412" s="1"/>
-      <c r="F412" s="1"/>
-    </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A413" s="1"/>
-      <c r="B413" s="1"/>
-      <c r="C413" s="1"/>
-      <c r="D413" s="1"/>
-      <c r="E413" s="1"/>
-      <c r="F413" s="1"/>
-    </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A414" s="1"/>
-      <c r="B414" s="1"/>
-      <c r="C414" s="1"/>
-      <c r="D414" s="1"/>
-      <c r="E414" s="1"/>
-      <c r="F414" s="1"/>
-    </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A415" s="1"/>
-      <c r="B415" s="1"/>
-      <c r="C415" s="1"/>
-      <c r="D415" s="1"/>
-      <c r="E415" s="1"/>
-      <c r="F415" s="1"/>
-    </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A416" s="1"/>
-      <c r="B416" s="1"/>
-      <c r="C416" s="1"/>
-      <c r="D416" s="1"/>
-      <c r="E416" s="1"/>
-      <c r="F416" s="1"/>
-    </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A417" s="1"/>
-      <c r="B417" s="1"/>
-      <c r="C417" s="1"/>
-      <c r="D417" s="1"/>
-      <c r="E417" s="1"/>
-      <c r="F417" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
     <mergeCell ref="A1:F2"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="E18:E22"/>
-    <mergeCell ref="F18:F22"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="E23:E27"/>
-    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>